<commit_message>
Change tax to 0.08
</commit_message>
<xml_diff>
--- a/public/samples/sample1.xlsx
+++ b/public/samples/sample1.xlsx
@@ -1927,6 +1927,102 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="38" fontId="5" fillId="0" borderId="55" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1941,180 +2037,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="distributed"/>
@@ -2147,6 +2069,15 @@
       <alignment vertical="distributed"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2166,11 +2097,80 @@
       <alignment vertical="distributed"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2243,24 +2243,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="156893184"/>
-        <c:axId val="156894720"/>
+        <c:axId val="193139840"/>
+        <c:axId val="193141376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="156893184"/>
+        <c:axId val="193139840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156894720"/>
+        <c:crossAx val="193141376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156894720"/>
+        <c:axId val="193141376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2268,7 +2268,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156893184"/>
+        <c:crossAx val="193139840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2280,7 +2280,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2654,8 +2654,8 @@
   </sheetPr>
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2671,145 +2671,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43.5" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1">
-      <c r="A2" s="67"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
+      <c r="A2" s="99"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
     </row>
     <row r="3" spans="1:11" ht="24" customHeight="1">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="68">
+      <c r="A3" s="99"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="100">
         <f ca="1">TODAY()</f>
         <v>41837</v>
       </c>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="18" customHeight="1">
-      <c r="A4" s="69"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
+      <c r="A4" s="101"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="70" t="s">
+      <c r="G4" s="102" t="s">
         <v>145</v>
       </c>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
     </row>
     <row r="5" spans="1:11" ht="18" customHeight="1">
-      <c r="A5" s="72"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="74" t="s">
         <v>146</v>
       </c>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
     </row>
     <row r="6" spans="1:11" ht="18" customHeight="1" thickBot="1">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
       <c r="D6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="72" t="s">
+      <c r="G6" s="74" t="s">
         <v>147</v>
       </c>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
     </row>
     <row r="7" spans="1:11" ht="18" customHeight="1">
-      <c r="A7" s="74"/>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
+      <c r="A7" s="93"/>
+      <c r="B7" s="93"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
     </row>
     <row r="8" spans="1:11" ht="18" customHeight="1">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
       <c r="E8" s="2"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="77" t="s">
+      <c r="G8" s="95" t="s">
         <v>148</v>
       </c>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="79"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="97"/>
     </row>
     <row r="9" spans="1:11" ht="18" customHeight="1">
-      <c r="A9" s="76"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
       <c r="E9" s="2"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="77" t="s">
+      <c r="G9" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="79"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="97"/>
     </row>
     <row r="10" spans="1:11" ht="18" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="80">
+      <c r="B10" s="85">
         <f ca="1">TODAY()+ 30</f>
         <v>41867</v>
       </c>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
       <c r="E10" s="2"/>
       <c r="F10" s="5"/>
       <c r="G10" s="2"/>
@@ -2821,17 +2821,17 @@
       <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="149" t="s">
+      <c r="B11" s="91" t="s">
         <v>147</v>
       </c>
-      <c r="C11" s="150"/>
-      <c r="D11" s="150"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
       <c r="E11" s="2"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="71" t="s">
+      <c r="G11" s="72" t="s">
         <v>150</v>
       </c>
-      <c r="H11" s="71"/>
+      <c r="H11" s="72"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
@@ -2839,9 +2839,9 @@
       <c r="A12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="150"/>
-      <c r="C12" s="150"/>
-      <c r="D12" s="150"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
       <c r="E12" s="2"/>
       <c r="F12" s="5"/>
       <c r="G12" s="2"/>
@@ -2853,540 +2853,519 @@
       <c r="A13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="80">
+      <c r="B13" s="85">
         <f ca="1">TODAY()+ 7</f>
         <v>41844</v>
       </c>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
       <c r="E13" s="2"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="23.25" customHeight="1">
       <c r="A14" s="8"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
       <c r="E14" s="2"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="83"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="18" customHeight="1" thickBot="1">
       <c r="A15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="85">
+      <c r="B15" s="88">
         <f>I35</f>
-        <v>9187</v>
-      </c>
-      <c r="C15" s="85"/>
-      <c r="D15" s="85"/>
+        <v>9450</v>
+      </c>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
       <c r="E15" s="2"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="83"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="83"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="21" customHeight="1">
-      <c r="A16" s="86"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="75"/>
-      <c r="J16" s="75"/>
+      <c r="A16" s="77"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="89"/>
+      <c r="J16" s="89"/>
     </row>
     <row r="17" spans="1:10" ht="18" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
       <c r="G17" s="11" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="87" t="s">
+      <c r="I17" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="87"/>
+      <c r="J17" s="90"/>
     </row>
     <row r="18" spans="1:10" ht="18" customHeight="1">
       <c r="A18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="81" t="s">
+      <c r="B18" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="81"/>
-      <c r="F18" s="81"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
       <c r="G18" s="13">
         <v>1</v>
       </c>
       <c r="H18" s="14">
         <v>2000</v>
       </c>
-      <c r="I18" s="82">
+      <c r="I18" s="75">
         <f>G18*H18</f>
         <v>2000</v>
       </c>
-      <c r="J18" s="82"/>
+      <c r="J18" s="75"/>
     </row>
     <row r="19" spans="1:10" ht="18" customHeight="1">
       <c r="A19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="81"/>
+      <c r="C19" s="83"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="83"/>
+      <c r="F19" s="83"/>
       <c r="G19" s="13">
         <v>2</v>
       </c>
       <c r="H19" s="14">
         <v>500</v>
       </c>
-      <c r="I19" s="82">
+      <c r="I19" s="75">
         <f t="shared" ref="I19:I32" si="0">G19*H19</f>
         <v>1000</v>
       </c>
-      <c r="J19" s="82"/>
+      <c r="J19" s="75"/>
     </row>
     <row r="20" spans="1:10" ht="18" customHeight="1">
       <c r="A20" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="81" t="s">
+      <c r="B20" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="81"/>
+      <c r="C20" s="83"/>
+      <c r="D20" s="83"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
       <c r="G20" s="13">
         <v>5</v>
       </c>
       <c r="H20" s="14">
         <v>300</v>
       </c>
-      <c r="I20" s="82">
+      <c r="I20" s="75">
         <f t="shared" si="0"/>
         <v>1500</v>
       </c>
-      <c r="J20" s="82"/>
+      <c r="J20" s="75"/>
     </row>
     <row r="21" spans="1:10" ht="18" customHeight="1">
       <c r="A21" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="81"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
+      <c r="E21" s="83"/>
+      <c r="F21" s="83"/>
       <c r="G21" s="13">
         <v>10</v>
       </c>
       <c r="H21" s="14">
         <v>200</v>
       </c>
-      <c r="I21" s="82">
+      <c r="I21" s="75">
         <f>G21*H21</f>
         <v>2000</v>
       </c>
-      <c r="J21" s="82"/>
+      <c r="J21" s="75"/>
     </row>
     <row r="22" spans="1:10" ht="18" customHeight="1">
       <c r="A22" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="81" t="s">
+      <c r="B22" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
-      <c r="F22" s="81"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
       <c r="G22" s="13">
         <v>15</v>
       </c>
       <c r="H22" s="14">
         <v>150</v>
       </c>
-      <c r="I22" s="82">
+      <c r="I22" s="75">
         <f t="shared" si="0"/>
         <v>2250</v>
       </c>
-      <c r="J22" s="82"/>
+      <c r="J22" s="75"/>
     </row>
     <row r="23" spans="1:10" ht="18" customHeight="1">
       <c r="A23" s="12"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
       <c r="G23" s="13"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="82">
+      <c r="I23" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J23" s="82"/>
+      <c r="J23" s="75"/>
     </row>
     <row r="24" spans="1:10" ht="18" customHeight="1">
       <c r="A24" s="12"/>
-      <c r="B24" s="81"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
       <c r="G24" s="13"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="82">
+      <c r="I24" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J24" s="82"/>
+      <c r="J24" s="75"/>
     </row>
     <row r="25" spans="1:10" ht="18" customHeight="1">
       <c r="A25" s="12"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
+      <c r="B25" s="83"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
       <c r="G25" s="13"/>
       <c r="H25" s="14"/>
-      <c r="I25" s="82">
+      <c r="I25" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J25" s="82"/>
+      <c r="J25" s="75"/>
     </row>
     <row r="26" spans="1:10" ht="18" customHeight="1">
       <c r="A26" s="12"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="81"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="83"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="83"/>
       <c r="G26" s="13"/>
       <c r="H26" s="14"/>
-      <c r="I26" s="82">
+      <c r="I26" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J26" s="82"/>
+      <c r="J26" s="75"/>
     </row>
     <row r="27" spans="1:10" ht="18" customHeight="1">
       <c r="A27" s="12"/>
-      <c r="B27" s="81"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
+      <c r="B27" s="83"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="83"/>
+      <c r="E27" s="83"/>
+      <c r="F27" s="83"/>
       <c r="G27" s="13"/>
       <c r="H27" s="14"/>
-      <c r="I27" s="82">
+      <c r="I27" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J27" s="82"/>
+      <c r="J27" s="75"/>
     </row>
     <row r="28" spans="1:10" ht="18" customHeight="1">
       <c r="A28" s="15"/>
-      <c r="B28" s="81"/>
-      <c r="C28" s="81"/>
-      <c r="D28" s="81"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
+      <c r="B28" s="83"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="83"/>
       <c r="G28" s="13"/>
       <c r="H28" s="14"/>
-      <c r="I28" s="82">
+      <c r="I28" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J28" s="82"/>
+      <c r="J28" s="75"/>
     </row>
     <row r="29" spans="1:10" ht="18" customHeight="1">
       <c r="A29" s="12"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="81"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
+      <c r="B29" s="83"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="83"/>
+      <c r="F29" s="83"/>
       <c r="G29" s="13"/>
       <c r="H29" s="14"/>
-      <c r="I29" s="82">
+      <c r="I29" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J29" s="82"/>
+      <c r="J29" s="75"/>
     </row>
     <row r="30" spans="1:10" ht="18" customHeight="1">
       <c r="A30" s="12"/>
-      <c r="B30" s="81"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="81"/>
-      <c r="F30" s="81"/>
+      <c r="B30" s="83"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="83"/>
       <c r="G30" s="13"/>
       <c r="H30" s="14"/>
-      <c r="I30" s="82">
+      <c r="I30" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J30" s="82"/>
+      <c r="J30" s="75"/>
     </row>
     <row r="31" spans="1:10" ht="18" customHeight="1">
       <c r="A31" s="12"/>
-      <c r="B31" s="81"/>
-      <c r="C31" s="81"/>
-      <c r="D31" s="81"/>
-      <c r="E31" s="81"/>
-      <c r="F31" s="81"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="83"/>
+      <c r="F31" s="83"/>
       <c r="G31" s="13"/>
       <c r="H31" s="14"/>
-      <c r="I31" s="82">
+      <c r="I31" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J31" s="82"/>
+      <c r="J31" s="75"/>
     </row>
     <row r="32" spans="1:10" ht="18" customHeight="1" thickBot="1">
       <c r="A32" s="16"/>
-      <c r="B32" s="88"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="88"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="81"/>
+      <c r="F32" s="81"/>
       <c r="G32" s="17"/>
       <c r="H32" s="18"/>
-      <c r="I32" s="82">
+      <c r="I32" s="75">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J32" s="82"/>
+      <c r="J32" s="75"/>
     </row>
     <row r="33" spans="1:10" ht="18" customHeight="1" thickTop="1">
       <c r="A33" s="19"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
+      <c r="B33" s="74"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
       <c r="G33" s="20"/>
       <c r="H33" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I33" s="89">
+      <c r="I33" s="82">
         <f>SUM(I18:J32)</f>
         <v>8750</v>
       </c>
-      <c r="J33" s="89"/>
+      <c r="J33" s="82"/>
     </row>
     <row r="34" spans="1:10" ht="18" customHeight="1">
       <c r="A34" s="19"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
       <c r="G34" s="20"/>
       <c r="H34" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I34" s="82">
-        <f>ROUNDDOWN(I33*0.05,0)</f>
-        <v>437</v>
-      </c>
-      <c r="J34" s="82"/>
+      <c r="I34" s="75">
+        <f>ROUNDDOWN(I33*0.08,0)</f>
+        <v>700</v>
+      </c>
+      <c r="J34" s="75"/>
     </row>
     <row r="35" spans="1:10" ht="18" customHeight="1">
       <c r="A35" s="19"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
+      <c r="B35" s="74"/>
+      <c r="C35" s="74"/>
+      <c r="D35" s="74"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="74"/>
       <c r="G35" s="20"/>
       <c r="H35" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="82">
+      <c r="I35" s="75">
         <f>SUM(I33:J34)</f>
-        <v>9187</v>
-      </c>
-      <c r="J35" s="82"/>
+        <v>9450</v>
+      </c>
+      <c r="J35" s="75"/>
     </row>
     <row r="36" spans="1:10" ht="18" customHeight="1">
-      <c r="A36" s="97"/>
-      <c r="B36" s="97"/>
-      <c r="C36" s="97"/>
-      <c r="D36" s="97"/>
-      <c r="E36" s="97"/>
-      <c r="F36" s="97"/>
-      <c r="G36" s="97"/>
-      <c r="H36" s="97"/>
-      <c r="I36" s="97"/>
-      <c r="J36" s="97"/>
+      <c r="A36" s="76"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
     </row>
     <row r="37" spans="1:10" ht="14.25">
       <c r="A37" s="23"/>
-      <c r="B37" s="86"/>
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
-      <c r="F37" s="86"/>
-      <c r="G37" s="86"/>
-      <c r="H37" s="86"/>
-      <c r="I37" s="86"/>
-      <c r="J37" s="86"/>
+      <c r="B37" s="77"/>
+      <c r="C37" s="77"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="77"/>
+      <c r="H37" s="77"/>
+      <c r="I37" s="77"/>
+      <c r="J37" s="77"/>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1">
-      <c r="A38" s="98" t="s">
+      <c r="A38" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="99"/>
-      <c r="C38" s="99"/>
-      <c r="D38" s="99"/>
-      <c r="E38" s="99"/>
-      <c r="F38" s="99"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="99"/>
-      <c r="I38" s="99"/>
-      <c r="J38" s="100"/>
+      <c r="B38" s="79"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="79"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="79"/>
+      <c r="H38" s="79"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="80"/>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1">
-      <c r="A39" s="90" t="s">
+      <c r="A39" s="66" t="s">
         <v>151</v>
       </c>
-      <c r="B39" s="91"/>
-      <c r="C39" s="91"/>
-      <c r="D39" s="91"/>
-      <c r="E39" s="91"/>
-      <c r="F39" s="91"/>
-      <c r="G39" s="91"/>
-      <c r="H39" s="91"/>
-      <c r="I39" s="91"/>
-      <c r="J39" s="92"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="67"/>
+      <c r="J39" s="68"/>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1">
-      <c r="A40" s="90"/>
-      <c r="B40" s="91"/>
-      <c r="C40" s="91"/>
-      <c r="D40" s="91"/>
-      <c r="E40" s="91"/>
-      <c r="F40" s="91"/>
-      <c r="G40" s="91"/>
-      <c r="H40" s="91"/>
-      <c r="I40" s="91"/>
-      <c r="J40" s="92"/>
+      <c r="A40" s="66"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="67"/>
+      <c r="D40" s="67"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="67"/>
+      <c r="J40" s="68"/>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1">
-      <c r="A41" s="90"/>
-      <c r="B41" s="91"/>
-      <c r="C41" s="91"/>
-      <c r="D41" s="91"/>
-      <c r="E41" s="91"/>
-      <c r="F41" s="91"/>
-      <c r="G41" s="91"/>
-      <c r="H41" s="91"/>
-      <c r="I41" s="91"/>
-      <c r="J41" s="92"/>
+      <c r="A41" s="66"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="67"/>
+      <c r="J41" s="68"/>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1">
-      <c r="A42" s="90"/>
-      <c r="B42" s="93"/>
-      <c r="C42" s="93"/>
-      <c r="D42" s="93"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="93"/>
-      <c r="G42" s="93"/>
-      <c r="H42" s="93"/>
-      <c r="I42" s="93"/>
-      <c r="J42" s="94"/>
+      <c r="A42" s="66"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="70"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="95"/>
-      <c r="B43" s="71"/>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
-      <c r="F43" s="71"/>
-      <c r="G43" s="71"/>
-      <c r="H43" s="71"/>
-      <c r="I43" s="71"/>
-      <c r="J43" s="96"/>
+      <c r="A43" s="71"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="72"/>
+      <c r="E43" s="72"/>
+      <c r="F43" s="72"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="72"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="A41:J41"/>
-    <mergeCell ref="A42:J42"/>
-    <mergeCell ref="A43:J43"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="A38:J38"/>
-    <mergeCell ref="A39:J39"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="B12:D12"/>
@@ -3401,25 +3380,46 @@
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="I18:J18"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="A43:J43"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="A38:J38"/>
+    <mergeCell ref="A39:J39"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -3458,18 +3458,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" customHeight="1" thickBot="1">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="149" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="102" t="s">
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="150" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
       <c r="J1" s="25" t="s">
         <v>30</v>
       </c>
@@ -3492,18 +3492,18 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="103" t="s">
+      <c r="A3" s="131" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="104"/>
-      <c r="C3" s="105" t="s">
+      <c r="B3" s="132"/>
+      <c r="C3" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="107"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="135"/>
       <c r="J3" s="31" t="s">
         <v>37</v>
       </c>
@@ -3515,10 +3515,10 @@
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="108" t="s">
+      <c r="A4" s="136" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="109"/>
+      <c r="B4" s="137"/>
       <c r="C4" s="34" t="s">
         <v>40</v>
       </c>
@@ -3540,16 +3540,16 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="110"/>
-      <c r="B5" s="111"/>
-      <c r="C5" s="112" t="s">
+      <c r="A5" s="138"/>
+      <c r="B5" s="139"/>
+      <c r="C5" s="140" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="113"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="113"/>
-      <c r="H5" s="114"/>
+      <c r="D5" s="141"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="141"/>
+      <c r="G5" s="141"/>
+      <c r="H5" s="142"/>
       <c r="J5" s="38" t="s">
         <v>45</v>
       </c>
@@ -3561,18 +3561,18 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="14.25" thickBot="1">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="119"/>
-      <c r="C6" s="120" t="s">
+      <c r="B6" s="127"/>
+      <c r="C6" s="128" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
-      <c r="G6" s="121"/>
-      <c r="H6" s="122"/>
+      <c r="D6" s="129"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="129"/>
+      <c r="G6" s="129"/>
+      <c r="H6" s="130"/>
       <c r="J6" s="38" t="s">
         <v>49</v>
       </c>
@@ -3609,16 +3609,16 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="103" t="s">
+      <c r="A9" s="131" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="104"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="106"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="107"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="134"/>
+      <c r="E9" s="134"/>
+      <c r="F9" s="134"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="135"/>
       <c r="J9" s="38" t="s">
         <v>56</v>
       </c>
@@ -3630,10 +3630,10 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="136" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="109"/>
+      <c r="B10" s="137"/>
       <c r="C10" s="34" t="s">
         <v>40</v>
       </c>
@@ -3653,14 +3653,14 @@
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="110"/>
-      <c r="B11" s="111"/>
-      <c r="C11" s="112"/>
-      <c r="D11" s="113"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="113"/>
-      <c r="G11" s="113"/>
-      <c r="H11" s="114"/>
+      <c r="A11" s="138"/>
+      <c r="B11" s="139"/>
+      <c r="C11" s="140"/>
+      <c r="D11" s="141"/>
+      <c r="E11" s="141"/>
+      <c r="F11" s="141"/>
+      <c r="G11" s="141"/>
+      <c r="H11" s="142"/>
       <c r="J11" s="38" t="s">
         <v>60</v>
       </c>
@@ -3670,16 +3670,16 @@
       <c r="L11" s="33"/>
     </row>
     <row r="12" spans="1:12" ht="14.25" thickBot="1">
-      <c r="A12" s="118" t="s">
+      <c r="A12" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="119"/>
-      <c r="C12" s="120"/>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="121"/>
-      <c r="H12" s="122"/>
+      <c r="B12" s="127"/>
+      <c r="C12" s="128"/>
+      <c r="D12" s="129"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="129"/>
+      <c r="G12" s="129"/>
+      <c r="H12" s="130"/>
       <c r="J12" s="38" t="s">
         <v>62</v>
       </c>
@@ -3701,11 +3701,11 @@
       <c r="B14" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="123" t="s">
+      <c r="C14" s="143" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="124"/>
-      <c r="E14" s="125"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="145"/>
       <c r="F14" s="40" t="s">
         <v>11</v>
       </c>
@@ -3730,12 +3730,12 @@
       <c r="B15" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="126" t="str">
+      <c r="C15" s="146" t="str">
         <f>IF(B15="","",VLOOKUP(B15,$J$2:$L$47,2))</f>
         <v>清涼スカッシュ</v>
       </c>
-      <c r="D15" s="127"/>
-      <c r="E15" s="128"/>
+      <c r="D15" s="147"/>
+      <c r="E15" s="148"/>
       <c r="F15" s="44">
         <v>5</v>
       </c>
@@ -3762,12 +3762,12 @@
       <c r="B16" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="115" t="str">
+      <c r="C16" s="116" t="str">
         <f>IF(B16="","",VLOOKUP(B16,$J$2:$L$47,2))</f>
         <v>パルメザンチーズ</v>
       </c>
-      <c r="D16" s="116"/>
-      <c r="E16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="118"/>
       <c r="F16" s="49">
         <v>10</v>
       </c>
@@ -3792,12 +3792,12 @@
         <v>3</v>
       </c>
       <c r="B17" s="48"/>
-      <c r="C17" s="115" t="str">
+      <c r="C17" s="116" t="str">
         <f>IF(B17="","",VLOOKUP(B17,$J$2:$L$47,2))</f>
         <v/>
       </c>
-      <c r="D17" s="116"/>
-      <c r="E17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="118"/>
       <c r="F17" s="49"/>
       <c r="G17" s="50" t="str">
         <f t="shared" ref="G17:G33" si="1">IF(F17="","",VLOOKUP(B17,$J$2:$L$47,3,FALSE))</f>
@@ -3820,12 +3820,12 @@
         <v>4</v>
       </c>
       <c r="B18" s="48"/>
-      <c r="C18" s="115" t="str">
+      <c r="C18" s="116" t="str">
         <f t="shared" ref="C18:C33" si="2">IF(B18="","",VLOOKUP(B18,$J$2:$L$47,2))</f>
         <v/>
       </c>
-      <c r="D18" s="116"/>
-      <c r="E18" s="117"/>
+      <c r="D18" s="117"/>
+      <c r="E18" s="118"/>
       <c r="F18" s="49"/>
       <c r="G18" s="50" t="str">
         <f t="shared" si="1"/>
@@ -3848,12 +3848,12 @@
         <v>5</v>
       </c>
       <c r="B19" s="48"/>
-      <c r="C19" s="115" t="str">
+      <c r="C19" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D19" s="116"/>
-      <c r="E19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="118"/>
       <c r="F19" s="49"/>
       <c r="G19" s="50" t="str">
         <f t="shared" si="1"/>
@@ -3876,12 +3876,12 @@
         <v>6</v>
       </c>
       <c r="B20" s="48"/>
-      <c r="C20" s="115" t="str">
+      <c r="C20" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D20" s="116"/>
-      <c r="E20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="118"/>
       <c r="F20" s="49"/>
       <c r="G20" s="50" t="str">
         <f t="shared" si="1"/>
@@ -3904,12 +3904,12 @@
         <v>7</v>
       </c>
       <c r="B21" s="48"/>
-      <c r="C21" s="115" t="str">
+      <c r="C21" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D21" s="116"/>
-      <c r="E21" s="117"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="118"/>
       <c r="F21" s="49"/>
       <c r="G21" s="50" t="str">
         <f t="shared" si="1"/>
@@ -3932,12 +3932,12 @@
         <v>8</v>
       </c>
       <c r="B22" s="48"/>
-      <c r="C22" s="115" t="str">
+      <c r="C22" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D22" s="116"/>
-      <c r="E22" s="117"/>
+      <c r="D22" s="117"/>
+      <c r="E22" s="118"/>
       <c r="F22" s="49"/>
       <c r="G22" s="50" t="str">
         <f t="shared" si="1"/>
@@ -3960,12 +3960,12 @@
         <v>9</v>
       </c>
       <c r="B23" s="48"/>
-      <c r="C23" s="115" t="str">
+      <c r="C23" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D23" s="116"/>
-      <c r="E23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="118"/>
       <c r="F23" s="49"/>
       <c r="G23" s="50" t="str">
         <f t="shared" si="1"/>
@@ -3988,12 +3988,12 @@
         <v>10</v>
       </c>
       <c r="B24" s="48"/>
-      <c r="C24" s="115" t="str">
+      <c r="C24" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D24" s="116"/>
-      <c r="E24" s="117"/>
+      <c r="D24" s="117"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="49"/>
       <c r="G24" s="50" t="str">
         <f t="shared" si="1"/>
@@ -4016,12 +4016,12 @@
         <v>11</v>
       </c>
       <c r="B25" s="48"/>
-      <c r="C25" s="115" t="str">
+      <c r="C25" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D25" s="116"/>
-      <c r="E25" s="117"/>
+      <c r="D25" s="117"/>
+      <c r="E25" s="118"/>
       <c r="F25" s="49"/>
       <c r="G25" s="50" t="str">
         <f t="shared" si="1"/>
@@ -4044,12 +4044,12 @@
         <v>12</v>
       </c>
       <c r="B26" s="48"/>
-      <c r="C26" s="115" t="str">
+      <c r="C26" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D26" s="116"/>
-      <c r="E26" s="117"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="118"/>
       <c r="F26" s="49"/>
       <c r="G26" s="50" t="str">
         <f t="shared" si="1"/>
@@ -4072,12 +4072,12 @@
         <v>13</v>
       </c>
       <c r="B27" s="48"/>
-      <c r="C27" s="115" t="str">
+      <c r="C27" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D27" s="116"/>
-      <c r="E27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="118"/>
       <c r="F27" s="49"/>
       <c r="G27" s="50" t="str">
         <f t="shared" si="1"/>
@@ -4100,12 +4100,12 @@
         <v>14</v>
       </c>
       <c r="B28" s="48"/>
-      <c r="C28" s="115" t="str">
+      <c r="C28" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D28" s="116"/>
-      <c r="E28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="118"/>
       <c r="F28" s="49"/>
       <c r="G28" s="50" t="str">
         <f t="shared" si="1"/>
@@ -4128,12 +4128,12 @@
         <v>15</v>
       </c>
       <c r="B29" s="48"/>
-      <c r="C29" s="115" t="str">
+      <c r="C29" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D29" s="116"/>
-      <c r="E29" s="117"/>
+      <c r="D29" s="117"/>
+      <c r="E29" s="118"/>
       <c r="F29" s="49"/>
       <c r="G29" s="50" t="str">
         <f t="shared" si="1"/>
@@ -4156,12 +4156,12 @@
         <v>16</v>
       </c>
       <c r="B30" s="48"/>
-      <c r="C30" s="115" t="str">
+      <c r="C30" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D30" s="116"/>
-      <c r="E30" s="117"/>
+      <c r="D30" s="117"/>
+      <c r="E30" s="118"/>
       <c r="F30" s="49"/>
       <c r="G30" s="50" t="str">
         <f t="shared" si="1"/>
@@ -4184,12 +4184,12 @@
         <v>17</v>
       </c>
       <c r="B31" s="48"/>
-      <c r="C31" s="115" t="str">
+      <c r="C31" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D31" s="116"/>
-      <c r="E31" s="117"/>
+      <c r="D31" s="117"/>
+      <c r="E31" s="118"/>
       <c r="F31" s="49"/>
       <c r="G31" s="50" t="str">
         <f t="shared" si="1"/>
@@ -4212,12 +4212,12 @@
         <v>18</v>
       </c>
       <c r="B32" s="48"/>
-      <c r="C32" s="115" t="str">
+      <c r="C32" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D32" s="116"/>
-      <c r="E32" s="117"/>
+      <c r="D32" s="117"/>
+      <c r="E32" s="118"/>
       <c r="F32" s="49"/>
       <c r="G32" s="50" t="str">
         <f t="shared" si="1"/>
@@ -4240,12 +4240,12 @@
         <v>19</v>
       </c>
       <c r="B33" s="48"/>
-      <c r="C33" s="115" t="str">
+      <c r="C33" s="116" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="D33" s="116"/>
-      <c r="E33" s="117"/>
+      <c r="D33" s="117"/>
+      <c r="E33" s="118"/>
       <c r="F33" s="49"/>
       <c r="G33" s="50" t="str">
         <f t="shared" si="1"/>
@@ -4268,12 +4268,12 @@
         <v>20</v>
       </c>
       <c r="B34" s="54"/>
-      <c r="C34" s="142" t="str">
+      <c r="C34" s="119" t="str">
         <f>IF(B34="","",VLOOKUP(B34,$J$2:$L$47,2))</f>
         <v/>
       </c>
-      <c r="D34" s="143"/>
-      <c r="E34" s="144"/>
+      <c r="D34" s="120"/>
+      <c r="E34" s="121"/>
       <c r="F34" s="55"/>
       <c r="G34" s="56" t="str">
         <f>IF(F34="","",VLOOKUP(B34,$J$2:$L$47,3,FALSE))</f>
@@ -4292,13 +4292,13 @@
       <c r="L34" s="33"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="C35" s="145" t="s">
+      <c r="C35" s="122" t="s">
         <v>111</v>
       </c>
-      <c r="D35" s="146"/>
-      <c r="E35" s="146"/>
-      <c r="F35" s="147"/>
-      <c r="G35" s="148"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="123"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="125"/>
       <c r="H35" s="58">
         <f>SUM(H15:H34)</f>
         <v>26000</v>
@@ -4312,13 +4312,13 @@
       <c r="L35" s="33"/>
     </row>
     <row r="36" spans="1:12" ht="14.25" thickBot="1">
-      <c r="C36" s="129" t="s">
+      <c r="C36" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="130"/>
-      <c r="E36" s="130"/>
-      <c r="F36" s="131"/>
-      <c r="G36" s="132"/>
+      <c r="D36" s="104"/>
+      <c r="E36" s="104"/>
+      <c r="F36" s="105"/>
+      <c r="G36" s="106"/>
       <c r="H36" s="59">
         <f>IF(H35&gt;=10000,500,0)</f>
         <v>500</v>
@@ -4332,13 +4332,13 @@
       <c r="L36" s="33"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="C37" s="133" t="s">
+      <c r="C37" s="107" t="s">
         <v>117</v>
       </c>
-      <c r="D37" s="134"/>
-      <c r="E37" s="134"/>
-      <c r="F37" s="134"/>
-      <c r="G37" s="135"/>
+      <c r="D37" s="108"/>
+      <c r="E37" s="108"/>
+      <c r="F37" s="108"/>
+      <c r="G37" s="109"/>
       <c r="H37" s="60">
         <f>H35+H36</f>
         <v>26500</v>
@@ -4352,13 +4352,13 @@
       <c r="L37" s="33"/>
     </row>
     <row r="38" spans="1:12" ht="14.25" thickBot="1">
-      <c r="C38" s="136" t="s">
+      <c r="C38" s="110" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="137"/>
-      <c r="E38" s="137"/>
-      <c r="F38" s="137"/>
-      <c r="G38" s="138"/>
+      <c r="D38" s="111"/>
+      <c r="E38" s="111"/>
+      <c r="F38" s="111"/>
+      <c r="G38" s="112"/>
       <c r="H38" s="61">
         <f>H37*0.08</f>
         <v>2120</v>
@@ -4372,13 +4372,13 @@
       <c r="L38" s="33"/>
     </row>
     <row r="39" spans="1:12" ht="14.25" thickBot="1">
-      <c r="C39" s="139" t="s">
+      <c r="C39" s="113" t="s">
         <v>123</v>
       </c>
-      <c r="D39" s="140"/>
-      <c r="E39" s="140"/>
-      <c r="F39" s="140"/>
-      <c r="G39" s="141"/>
+      <c r="D39" s="114"/>
+      <c r="E39" s="114"/>
+      <c r="F39" s="114"/>
+      <c r="G39" s="115"/>
       <c r="H39" s="62">
         <f>H37+H38</f>
         <v>28620</v>
@@ -4456,16 +4456,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="C36:G36"/>
-    <mergeCell ref="C37:G37"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="C30:E30"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="C33:E33"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
     <mergeCell ref="C29:E29"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="C19:E19"/>
@@ -4478,24 +4486,16 @@
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A4:B5"/>
-    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="C37:G37"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="C33:E33"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C35:G35"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="3">

</xml_diff>